<commit_message>
Update Round1 model performance - Nisal.xlsx
</commit_message>
<xml_diff>
--- a/results/Round1 model performance - Nisal.xlsx
+++ b/results/Round1 model performance - Nisal.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9215E1B-F07E-49C7-A8B0-B38F554E462E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19419EF-A470-47B2-A33C-192A164F4F86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="2690" windowWidth="14400" windowHeight="7510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Model</t>
   </si>
@@ -75,6 +75,27 @@
   </si>
   <si>
     <t>OneHot</t>
+  </si>
+  <si>
+    <t>CV 5 fold Train/Val</t>
+  </si>
+  <si>
+    <t>LGBM</t>
+  </si>
+  <si>
+    <t>max_depth=10, class_weight='balanced'</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>preprocessed_train_val_Mar13_0130pm_label_enc</t>
+  </si>
+  <si>
+    <t>CatBoostClassifier</t>
+  </si>
+  <si>
+    <t>max_depth=10, auto_class_weights='Balanced', n_estimators=10</t>
   </si>
 </sst>
 </file>
@@ -414,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -425,12 +446,14 @@
     <col min="1" max="1" width="16.54296875" customWidth="1"/>
     <col min="2" max="2" width="20.81640625" customWidth="1"/>
     <col min="3" max="3" width="21.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.1796875" style="2"/>
-    <col min="7" max="7" width="8.7265625" style="2"/>
+    <col min="4" max="4" width="49.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1796875" style="2"/>
+    <col min="8" max="8" width="8.7265625" style="2"/>
+    <col min="9" max="9" width="17.90625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -443,17 +466,23 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -466,14 +495,15 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1"/>
+      <c r="F2" s="2">
         <v>0.3715</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>0.36149999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -486,14 +516,15 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1"/>
+      <c r="F3" s="2">
         <v>0.37386999999999998</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>0.64278599999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -506,14 +537,15 @@
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1"/>
+      <c r="F4" s="2">
         <v>0.35886000000000001</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>0.42703999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -526,17 +558,18 @@
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1"/>
+      <c r="F5" s="2">
         <v>0.51205000000000001</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>0.30459999999999998</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>0.25644099999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -549,14 +582,43 @@
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1"/>
+      <c r="F6" s="2">
         <v>0.52095999999999998</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>0.30480000000000002</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>0.25669999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.38839000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.35049999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>